<commit_message>
Change pcb to have parallel work
</commit_message>
<xml_diff>
--- a/Circuit diagram/PABSv6.0_BOM.xlsx
+++ b/Circuit diagram/PABSv6.0_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Comment</t>
   </si>
@@ -91,9 +91,6 @@
     <t>50Ω</t>
   </si>
   <si>
-    <t>R1-10</t>
-  </si>
-  <si>
     <t>1KΩ</t>
   </si>
   <si>
@@ -134,6 +131,30 @@
   </si>
   <si>
     <t>R21-23</t>
+  </si>
+  <si>
+    <t>R1-10,R52</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>R51, R53</t>
+  </si>
+  <si>
+    <t>C8545</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>C17936</t>
   </si>
 </sst>
 </file>
@@ -514,7 +535,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -550,7 +571,7 @@
         <v>1206</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -562,10 +583,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -576,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -587,41 +608,41 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>1206</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>1206</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="2">
         <v>1206</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -629,19 +650,42 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2">
         <v>1206</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1206</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="6"/>

</xml_diff>